<commit_message>
Modified code with User Creation
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -4,54 +4,78 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="96" windowWidth="22980" windowHeight="9288"/>
+    <workbookView xWindow="0" yWindow="2448" windowWidth="14328" windowHeight="6096"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:M19"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>loes4</t>
+  </si>
+  <si>
+    <t>loes5</t>
+  </si>
+  <si>
+    <t>loes6</t>
+  </si>
+  <si>
+    <t>loes7</t>
+  </si>
+  <si>
+    <t>loes8</t>
+  </si>
+  <si>
+    <t>loes9</t>
+  </si>
+  <si>
+    <t>loes10</t>
+  </si>
+  <si>
+    <t>loes11</t>
+  </si>
+  <si>
+    <t>loes12</t>
+  </si>
+  <si>
+    <t>loes2</t>
+  </si>
+  <si>
+    <t>loes3</t>
+  </si>
+  <si>
+    <t>loes13</t>
+  </si>
+  <si>
+    <t>loes14</t>
+  </si>
+  <si>
+    <t>loes15</t>
+  </si>
+  <si>
+    <t>loes16</t>
+  </si>
+  <si>
+    <t>loes17</t>
+  </si>
+  <si>
+    <t>loes18</t>
+  </si>
+  <si>
+    <t>loes19</t>
+  </si>
+  <si>
+    <t>loes20</t>
+  </si>
   <si>
     <t>loes1</t>
-  </si>
-  <si>
-    <t>loes2</t>
-  </si>
-  <si>
-    <t>loes3</t>
-  </si>
-  <si>
-    <t>loes4</t>
-  </si>
-  <si>
-    <t>loes5</t>
-  </si>
-  <si>
-    <t>loes6</t>
-  </si>
-  <si>
-    <t>loes7</t>
-  </si>
-  <si>
-    <t>loes8</t>
-  </si>
-  <si>
-    <t>loes9</t>
-  </si>
-  <si>
-    <t>loes10</t>
-  </si>
-  <si>
-    <t>loes11</t>
-  </si>
-  <si>
-    <t>loes12</t>
   </si>
 </sst>
 </file>
@@ -87,8 +111,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,73 +415,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -473,16 +562,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>